<commit_message>
KISS-29: cmake/doc/CMake Inventory.xlsx: Added: column F, G: CMake for tools/utils, column H, I: CMake for Delft3D4
</commit_message>
<xml_diff>
--- a/src/cmake/doc/CMake Inventory.xlsx
+++ b/src/cmake/doc/CMake Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN_Repos\OSS\src\cmake\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\oss\src\cmake\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9CAD00-33C7-4331-9C64-AAFD819BA6F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F479B-3ECD-41B9-9732-1F2628ECB869}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="1965" windowWidth="28800" windowHeight="15435" xr2:uid="{7C701F35-EF14-4830-B541-23814411E7FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7C701F35-EF14-4830-B541-23814411E7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Repository" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="174">
   <si>
     <t xml:space="preserve"> Component</t>
   </si>
@@ -532,6 +532,27 @@
   </si>
   <si>
     <t>Note: only  the Fortran lib was considered</t>
+  </si>
+  <si>
+    <t>CMakeLists19-10-2021</t>
+  </si>
+  <si>
+    <t>CMakeLists 2022</t>
+  </si>
+  <si>
+    <t>Everything related to flow2d3d</t>
+  </si>
+  <si>
+    <t>Done; check</t>
+  </si>
+  <si>
+    <t>Low priority</t>
+  </si>
+  <si>
+    <t>! Is the dll created?</t>
+  </si>
+  <si>
+    <t>!Check that it works</t>
   </si>
 </sst>
 </file>
@@ -563,7 +584,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -571,21 +592,612 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -921,23 +1533,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A47A33-32B4-4075-AB2F-D5C67F77139F}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="H99" sqref="H99:H102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -953,8 +1569,20 @@
       <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -967,8 +1595,14 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -979,7 +1613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -987,7 +1621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -995,7 +1629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1003,7 +1637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1011,7 +1645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1022,7 +1656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -1030,23 +1664,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1056,72 +1702,99 @@
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -1132,15 +1805,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>28</v>
       </c>
@@ -1148,7 +1827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>29</v>
       </c>
@@ -1156,7 +1835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>30</v>
       </c>
@@ -1164,7 +1843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>31</v>
       </c>
@@ -1175,15 +1854,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>35</v>
       </c>
@@ -1191,7 +1876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>38</v>
       </c>
@@ -1207,7 +1892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>39</v>
       </c>
@@ -1215,7 +1900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>40</v>
       </c>
@@ -1223,7 +1908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>41</v>
       </c>
@@ -1231,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>42</v>
       </c>
@@ -1239,7 +1924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>43</v>
       </c>
@@ -1247,7 +1932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>44</v>
       </c>
@@ -1255,7 +1940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>45</v>
       </c>
@@ -1266,7 +1951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>18</v>
       </c>
@@ -1274,7 +1959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>20</v>
       </c>
@@ -1282,7 +1967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
         <v>22</v>
       </c>
@@ -1290,15 +1975,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1308,16 +1994,23 @@
       <c r="D42" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="H42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F43" s="5"/>
+      <c r="H43" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -1330,16 +2023,28 @@
       <c r="D44" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
         <v>52</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>53</v>
       </c>
@@ -1349,19 +2054,31 @@
       <c r="D46" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="F46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1374,8 +2091,11 @@
       <c r="D48" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H48" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>58</v>
       </c>
@@ -1386,15 +2106,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>59</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F50" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>60</v>
       </c>
@@ -1402,7 +2125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>61</v>
       </c>
@@ -1410,7 +2133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>62</v>
       </c>
@@ -1421,7 +2144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>63</v>
       </c>
@@ -1432,7 +2155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>64</v>
       </c>
@@ -1440,7 +2163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
         <v>65</v>
       </c>
@@ -1448,7 +2171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>66</v>
       </c>
@@ -1456,7 +2179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>67</v>
       </c>
@@ -1466,16 +2189,28 @@
       <c r="D58" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>68</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>69</v>
       </c>
@@ -1486,7 +2221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>70</v>
       </c>
@@ -1494,7 +2229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>71</v>
       </c>
@@ -1502,7 +2237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>72</v>
       </c>
@@ -1513,7 +2248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>73</v>
       </c>
@@ -1523,16 +2258,28 @@
       <c r="D64" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>74</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G65" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>75</v>
       </c>
@@ -1543,7 +2290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>76</v>
       </c>
@@ -1556,8 +2303,14 @@
       <c r="E67" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>78</v>
       </c>
@@ -1568,7 +2321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>79</v>
       </c>
@@ -1579,7 +2332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>81</v>
       </c>
@@ -1589,8 +2342,14 @@
       <c r="D70" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>82</v>
       </c>
@@ -1601,7 +2360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>83</v>
       </c>
@@ -1611,24 +2370,42 @@
       <c r="D72" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
         <v>85</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
+      <c r="F73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G73" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -1641,8 +2418,14 @@
       <c r="D75" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
         <v>90</v>
       </c>
@@ -1650,7 +2433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>91</v>
       </c>
@@ -1661,7 +2444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
         <v>92</v>
       </c>
@@ -1669,7 +2452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>93</v>
       </c>
@@ -1677,7 +2460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>94</v>
       </c>
@@ -1688,7 +2471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
         <v>96</v>
       </c>
@@ -1696,7 +2479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
         <v>97</v>
       </c>
@@ -1704,7 +2487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
         <v>98</v>
       </c>
@@ -1712,7 +2495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
         <v>99</v>
       </c>
@@ -1720,15 +2503,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+    <row r="85" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -1741,24 +2525,33 @@
       <c r="D86" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H86" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
         <v>103</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H87" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
         <v>104</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H88" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>105</v>
       </c>
@@ -1769,7 +2562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>106</v>
       </c>
@@ -1780,7 +2573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
         <v>107</v>
       </c>
@@ -1788,7 +2581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>109</v>
       </c>
@@ -1798,24 +2591,33 @@
       <c r="D92" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H92" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
         <v>110</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H93" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
         <v>111</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H94" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>112</v>
       </c>
@@ -1825,24 +2627,33 @@
       <c r="D95" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H95" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
         <v>113</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H96" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
         <v>114</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H97" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>115</v>
       </c>
@@ -1852,8 +2663,11 @@
       <c r="D98" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>116</v>
       </c>
@@ -1863,8 +2677,11 @@
       <c r="D99" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H99" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>117</v>
       </c>
@@ -1874,8 +2691,11 @@
       <c r="D100" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H100" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>118</v>
       </c>
@@ -1885,16 +2705,22 @@
       <c r="D101" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H101" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
         <v>119</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H102" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>120</v>
       </c>
@@ -1905,15 +2731,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C104" t="s">
         <v>121</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G104" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>122</v>
       </c>
@@ -1924,7 +2756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
         <v>124</v>
       </c>
@@ -1932,15 +2764,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+    <row r="107" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D107" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>126</v>
       </c>
@@ -1954,18 +2787,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+    <row r="109" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D109" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>129</v>
       </c>
@@ -1977,7 +2811,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>131</v>
       </c>
@@ -1986,7 +2820,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>132</v>
       </c>
@@ -1995,7 +2829,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>133</v>
       </c>
@@ -2006,7 +2840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>135</v>
       </c>
@@ -2017,7 +2851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>136</v>
       </c>
@@ -2028,7 +2862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C116" t="s">
         <v>138</v>
       </c>
@@ -2036,7 +2870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>139</v>
       </c>
@@ -2045,7 +2879,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>140</v>
       </c>
@@ -2054,7 +2888,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>141</v>
       </c>
@@ -2065,7 +2899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>142</v>
       </c>
@@ -2074,7 +2908,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>143</v>
       </c>
@@ -2085,7 +2919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>144</v>
       </c>
@@ -2096,7 +2930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
         <v>146</v>
       </c>
@@ -2104,7 +2938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>147</v>
       </c>
@@ -2115,7 +2949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>149</v>
       </c>
@@ -2124,7 +2958,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>150</v>
       </c>
@@ -2133,7 +2967,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>151</v>
       </c>
@@ -2144,7 +2978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>152</v>
       </c>
@@ -2153,7 +2987,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>153</v>
       </c>
@@ -2164,7 +2998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>154</v>
       </c>
@@ -2175,7 +3009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>155</v>
       </c>
@@ -2186,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>156</v>
       </c>
@@ -2195,7 +3029,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>157</v>
       </c>
@@ -2206,7 +3040,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>158</v>
       </c>
@@ -2215,7 +3049,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>159</v>
       </c>
@@ -2224,7 +3058,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>160</v>
       </c>
@@ -2233,7 +3067,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>161</v>
       </c>
@@ -2242,7 +3076,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>162</v>
       </c>
@@ -2251,7 +3085,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>163</v>
       </c>
@@ -2262,7 +3096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>165</v>
       </c>
@@ -2271,7 +3105,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>164</v>
       </c>
@@ -2284,11 +3118,195 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D141">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F11">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H20">
+    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42:H43">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F44:F46">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F47">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F58">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F104">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F59">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F64">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F65">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F70">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F72:F74">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F75">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H86:H88">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H92:H97">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F98">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H99:H102">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2564,16 +3582,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A51D89-B7C2-4C26-9689-E91B9B95F575}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="40f483c7-5140-4967-803d-fe03d92f7b49"/>
     <ds:schemaRef ds:uri="1f5afa80-5dac-40c9-bf44-cf66b310199c"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
KISS-29: Update excel file entries
</commit_message>
<xml_diff>
--- a/src/cmake/doc/CMake Inventory.xlsx
+++ b/src/cmake/doc/CMake Inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\oss\src\cmake\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ENGINES\delft3d\trunk\src\cmake\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2F479B-3ECD-41B9-9732-1F2628ECB869}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894F40D9-2ABD-4E5D-8088-1E49B493EFDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7C701F35-EF14-4830-B541-23814411E7FF}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{7C701F35-EF14-4830-B541-23814411E7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Repository" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="172">
   <si>
     <t xml:space="preserve"> Component</t>
   </si>
@@ -547,12 +547,6 @@
   </si>
   <si>
     <t>Low priority</t>
-  </si>
-  <si>
-    <t>! Is the dll created?</t>
-  </si>
-  <si>
-    <t>!Check that it works</t>
   </si>
 </sst>
 </file>
@@ -902,6 +896,19 @@
       <font>
         <b/>
         <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -927,6 +934,18 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
         <color theme="0"/>
       </font>
@@ -1195,31 +1214,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1536,24 +1530,24 @@
   <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H99" sqref="H99:H102"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1582,7 +1576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1596,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1613,7 +1607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1621,7 +1615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>8</v>
       </c>
@@ -1637,7 +1631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>9</v>
       </c>
@@ -1645,7 +1639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -1656,7 +1650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>13</v>
       </c>
@@ -1664,7 +1658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -1678,7 +1672,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>15</v>
       </c>
@@ -1692,7 +1686,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -1706,7 +1700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>16</v>
       </c>
@@ -1717,7 +1711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -1728,7 +1722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>19</v>
       </c>
@@ -1739,7 +1733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>20</v>
       </c>
@@ -1750,7 +1744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>21</v>
       </c>
@@ -1761,7 +1755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>23</v>
       </c>
@@ -1783,7 +1777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>24</v>
       </c>
@@ -1794,7 +1788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -1805,7 +1799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>27</v>
       </c>
@@ -1819,7 +1813,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>28</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>29</v>
       </c>
@@ -1835,7 +1829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>30</v>
       </c>
@@ -1843,7 +1837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>31</v>
       </c>
@@ -1854,7 +1848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>37</v>
       </c>
@@ -1868,7 +1862,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>35</v>
       </c>
@@ -1876,7 +1870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>36</v>
       </c>
@@ -1884,7 +1878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>38</v>
       </c>
@@ -1892,7 +1886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>39</v>
       </c>
@@ -1900,7 +1894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>40</v>
       </c>
@@ -1908,7 +1902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>41</v>
       </c>
@@ -1916,7 +1910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>42</v>
       </c>
@@ -1924,7 +1918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>43</v>
       </c>
@@ -1932,7 +1926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>44</v>
       </c>
@@ -1940,7 +1934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>45</v>
       </c>
@@ -1951,7 +1945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>18</v>
       </c>
@@ -1959,7 +1953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>20</v>
       </c>
@@ -1967,7 +1961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>22</v>
       </c>
@@ -1975,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="4" t="s">
         <v>46</v>
       </c>
@@ -1984,7 +1978,7 @@
       </c>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1998,7 +1992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>49</v>
       </c>
@@ -2010,7 +2004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2030,7 +2024,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>52</v>
       </c>
@@ -2044,7 +2038,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>53</v>
       </c>
@@ -2061,7 +2055,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>55</v>
       </c>
@@ -2078,7 +2072,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2095,7 +2089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>58</v>
       </c>
@@ -2106,7 +2100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>59</v>
       </c>
@@ -2117,7 +2111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>60</v>
       </c>
@@ -2125,7 +2119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>61</v>
       </c>
@@ -2133,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>62</v>
       </c>
@@ -2144,7 +2138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>63</v>
       </c>
@@ -2155,7 +2149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>64</v>
       </c>
@@ -2163,7 +2157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>65</v>
       </c>
@@ -2171,7 +2165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>66</v>
       </c>
@@ -2179,7 +2173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>67</v>
       </c>
@@ -2189,14 +2183,8 @@
       <c r="D58" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>68</v>
       </c>
@@ -2210,7 +2198,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>69</v>
       </c>
@@ -2221,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>70</v>
       </c>
@@ -2229,7 +2217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>71</v>
       </c>
@@ -2237,7 +2225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>72</v>
       </c>
@@ -2248,7 +2236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>73</v>
       </c>
@@ -2258,14 +2246,9 @@
       <c r="D64" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>74</v>
       </c>
@@ -2279,7 +2262,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>75</v>
       </c>
@@ -2290,7 +2273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>76</v>
       </c>
@@ -2303,14 +2286,9 @@
       <c r="E67" t="s">
         <v>166</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>78</v>
       </c>
@@ -2320,8 +2298,9 @@
       <c r="D68" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>79</v>
       </c>
@@ -2331,8 +2310,9 @@
       <c r="D69" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>81</v>
       </c>
@@ -2342,14 +2322,9 @@
       <c r="D70" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>82</v>
       </c>
@@ -2360,7 +2335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>83</v>
       </c>
@@ -2377,7 +2352,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>85</v>
       </c>
@@ -2391,7 +2366,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C74" s="4" t="s">
         <v>86</v>
       </c>
@@ -2405,7 +2380,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -2416,16 +2391,10 @@
         <v>89</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G75" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>90</v>
       </c>
@@ -2433,7 +2402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>91</v>
       </c>
@@ -2444,7 +2413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>92</v>
       </c>
@@ -2452,7 +2421,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>93</v>
       </c>
@@ -2460,7 +2429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>94</v>
       </c>
@@ -2471,7 +2440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>96</v>
       </c>
@@ -2479,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>97</v>
       </c>
@@ -2487,7 +2456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>98</v>
       </c>
@@ -2495,7 +2464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>99</v>
       </c>
@@ -2503,7 +2472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C85" s="4" t="s">
         <v>100</v>
       </c>
@@ -2512,7 +2481,7 @@
       </c>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -2529,7 +2498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>103</v>
       </c>
@@ -2540,7 +2509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
         <v>104</v>
       </c>
@@ -2551,7 +2520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>105</v>
       </c>
@@ -2562,7 +2531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>106</v>
       </c>
@@ -2573,15 +2542,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
         <v>107</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>109</v>
       </c>
@@ -2591,33 +2561,36 @@
       <c r="D92" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F92"/>
       <c r="H92" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>110</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F93"/>
       <c r="H93" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>111</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F94"/>
       <c r="H94" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>112</v>
       </c>
@@ -2627,33 +2600,36 @@
       <c r="D95" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F95"/>
       <c r="H95" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
         <v>113</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F96"/>
       <c r="H96" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>114</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F97"/>
       <c r="H97" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>115</v>
       </c>
@@ -2663,11 +2639,9 @@
       <c r="D98" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F98" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>116</v>
       </c>
@@ -2677,11 +2651,12 @@
       <c r="D99" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F99"/>
       <c r="H99" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>117</v>
       </c>
@@ -2691,11 +2666,12 @@
       <c r="D100" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F100"/>
       <c r="H100" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>118</v>
       </c>
@@ -2705,22 +2681,24 @@
       <c r="D101" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F101"/>
       <c r="H101" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
         <v>119</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F102"/>
       <c r="H102" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>120</v>
       </c>
@@ -2730,22 +2708,18 @@
       <c r="D103" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
         <v>121</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F104" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G104" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>122</v>
       </c>
@@ -2755,16 +2729,18 @@
       <c r="D105" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
         <v>124</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C107" s="4" t="s">
         <v>125</v>
       </c>
@@ -2773,7 +2749,7 @@
       </c>
       <c r="F107" s="5"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>126</v>
       </c>
@@ -2787,7 +2763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="s">
         <v>128</v>
       </c>
@@ -2799,7 +2775,7 @@
       </c>
       <c r="F109" s="5"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>129</v>
       </c>
@@ -2811,7 +2787,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>131</v>
       </c>
@@ -2820,7 +2796,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>132</v>
       </c>
@@ -2829,7 +2805,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>133</v>
       </c>
@@ -2840,7 +2816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>135</v>
       </c>
@@ -2851,7 +2827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>136</v>
       </c>
@@ -2862,7 +2838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
         <v>138</v>
       </c>
@@ -2870,7 +2846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>139</v>
       </c>
@@ -2879,7 +2855,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>140</v>
       </c>
@@ -2888,7 +2864,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>141</v>
       </c>
@@ -2899,7 +2875,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>142</v>
       </c>
@@ -2908,7 +2884,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>143</v>
       </c>
@@ -2919,7 +2895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>144</v>
       </c>
@@ -2930,7 +2906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
         <v>146</v>
       </c>
@@ -2938,7 +2914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>147</v>
       </c>
@@ -2949,7 +2925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>149</v>
       </c>
@@ -2958,7 +2934,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>150</v>
       </c>
@@ -2967,7 +2943,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>151</v>
       </c>
@@ -2978,7 +2954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>152</v>
       </c>
@@ -2987,7 +2963,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>153</v>
       </c>
@@ -2998,7 +2974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>154</v>
       </c>
@@ -3009,7 +2985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>155</v>
       </c>
@@ -3020,7 +2996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>156</v>
       </c>
@@ -3029,7 +3005,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>157</v>
       </c>
@@ -3040,7 +3016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>158</v>
       </c>
@@ -3049,7 +3025,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>159</v>
       </c>
@@ -3058,7 +3034,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>160</v>
       </c>
@@ -3067,7 +3043,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>161</v>
       </c>
@@ -3076,7 +3052,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>162</v>
       </c>
@@ -3085,7 +3061,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>163</v>
       </c>
@@ -3096,7 +3072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>165</v>
       </c>
@@ -3105,7 +3081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>164</v>
       </c>
@@ -3118,11 +3094,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D141">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
       <formula>"Y"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:F11">
@@ -3213,11 +3189,11 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F104">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+  <conditionalFormatting sqref="F96">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3229,35 +3205,11 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F64">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F65">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"N"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>"Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F70">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"N"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3269,7 +3221,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F75">
+  <conditionalFormatting sqref="D75">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
KISS-29: Restore delwaq2, update cmake inventory.xlsx
</commit_message>
<xml_diff>
--- a/src/cmake/doc/CMake Inventory.xlsx
+++ b/src/cmake/doc/CMake Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ENGINES\delft3d\trunk\src\cmake\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894F40D9-2ABD-4E5D-8088-1E49B493EFDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21BBD63-2962-4CC4-AAEB-225E69F6B05A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{7C701F35-EF14-4830-B541-23814411E7FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7C701F35-EF14-4830-B541-23814411E7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Repository" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="172">
   <si>
     <t xml:space="preserve"> Component</t>
   </si>
@@ -616,82 +616,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="42">
     <dxf>
       <font>
         <b/>
@@ -1530,8 +1455,8 @@
   <dimension ref="A1:I141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,13 +1729,7 @@
         <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -3094,122 +3013,122 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D141">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10:F11">
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H20">
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42:H43">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F44:F46">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F50">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F96">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F65">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3267,6 +3186,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EFB54AE667A1B47810A66C50A7392AA" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7370bee7a5aadbe7c184359a945c98c1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40f483c7-5140-4967-803d-fe03d92f7b49" xmlns:ns4="1f5afa80-5dac-40c9-bf44-cf66b310199c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d053b80db4e91b8a1143f0c858ac7bd" ns3:_="" ns4:_="">
     <xsd:import namespace="40f483c7-5140-4967-803d-fe03d92f7b49"/>
@@ -3489,22 +3423,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A51D89-B7C2-4C26-9689-E91B9B95F575}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="40f483c7-5140-4967-803d-fe03d92f7b49"/>
+    <ds:schemaRef ds:uri="1f5afa80-5dac-40c9-bf44-cf66b310199c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7718D3E4-3594-40B1-AA27-85EE352ADFF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76384A7A-CC49-44BF-B9B6-F6F8020BB114}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3521,29 +3465,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7718D3E4-3594-40B1-AA27-85EE352ADFF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91A51D89-B7C2-4C26-9689-E91B9B95F575}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="40f483c7-5140-4967-803d-fe03d92f7b49"/>
-    <ds:schemaRef ds:uri="1f5afa80-5dac-40c9-bf44-cf66b310199c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>